<commit_message>
Changes done in testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestData.xlsx
+++ b/src/test/resources/testdata/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SHAHNAWAZ KHAN\eclipse-workspace\OrangeHRMProject\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Selenium-E2E-Test-Framework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCA189E-6D59-4FE8-A5B8-CABC0D192FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803BD6A3-FA07-43E0-BDE6-23E237E4068A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5856" yWindow="4728" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validLoginData" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
     <t>admin</t>
   </si>
   <si>
-    <t>shahnawaz</t>
-  </si>
-  <si>
-    <t>Attitude665665@</t>
-  </si>
-  <si>
     <t>emp_id</t>
   </si>
   <si>
@@ -51,6 +45,12 @@
   </si>
   <si>
     <t>Asif</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,15 +400,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{EDF8E963-0E9A-41BE-A2D6-F22E8D0F9ED9}"/>
+    <hyperlink ref="B2" r:id="rId1" display="Attitude665665@" xr:uid="{EDF8E963-0E9A-41BE-A2D6-F22E8D0F9ED9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -418,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{957A83F8-EFD9-4830-A730-B0568945854E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -426,10 +426,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -437,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>